<commit_message>
Vinayak Change to add all items in cart.
</commit_message>
<xml_diff>
--- a/src/test/java/resources_Utility/Greenkart_Test_Cases.xlsx
+++ b/src/test/java/resources_Utility/Greenkart_Test_Cases.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="23565" windowHeight="5610" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16740" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="TestData" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>Test ID</t>
   </si>
@@ -139,13 +139,19 @@
   </si>
   <si>
     <t>ajay</t>
+  </si>
+  <si>
+    <t>GK_016_Test</t>
+  </si>
+  <si>
+    <t>Verify user is able to add all vegitables.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,7 +302,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -331,7 +336,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -507,14 +511,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="107.5703125" customWidth="1"/>
@@ -524,28 +528,28 @@
     <col min="6" max="6" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18.75">
       <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18.75">
       <c r="A3" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="18.75">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="21">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -565,7 +569,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -576,7 +580,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -587,7 +591,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -598,7 +602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -609,7 +613,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -620,7 +624,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -631,7 +635,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -642,7 +646,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -653,7 +657,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -664,7 +668,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -675,7 +679,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -686,7 +690,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -697,7 +701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -708,7 +712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -719,7 +723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -728,6 +732,14 @@
       </c>
       <c r="F20" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -741,16 +753,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -761,12 +773,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>